<commit_message>
fix links to data source
</commit_message>
<xml_diff>
--- a/week-2/Exercises/2-2-A-building-charts-exercises.xlsx
+++ b/week-2/Exercises/2-2-A-building-charts-exercises.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\data-analytics-lectures\week-2\Exercises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George Mount\Documents\GitHub\data-analytics-lectures\week-2\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC496895-6E33-4E77-ACFB-9EDCD4C19CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="applicants" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,9 +34,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="11">
   <si>
     <t xml:space="preserve">Data source: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.rdocumentation.org/packages/babynames/versions/1.0.0 </t>
   </si>
   <si>
     <t>year</t>
@@ -66,11 +62,14 @@
   <si>
     <t>3. Total number of male versus female applications since 2015</t>
   </si>
+  <si>
+    <t>https://www.ssa.gov/oact/babynames/numberUSbirths.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,12 +130,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7B74F6A-844E-4C2E-9241-E7F5F1A744EA}" name="applicants" displayName="applicants" ref="A1:C277" totalsRowShown="0">
-  <autoFilter ref="A1:C277" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="applicants" displayName="applicants" ref="A1:C277" totalsRowShown="0">
+  <autoFilter ref="A1:C277"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C98016AC-A828-4F74-BA44-0BBFA14529BD}" name="year"/>
-    <tableColumn id="2" xr3:uid="{2016CC4F-D7A2-42D0-BE46-D57291CDBE64}" name="sex"/>
-    <tableColumn id="3" xr3:uid="{D2C5F70C-CAD7-441C-BC2D-C85D3D2DC9D9}" name="n_all"/>
+    <tableColumn id="1" name="year"/>
+    <tableColumn id="2" name="sex"/>
+    <tableColumn id="3" name="n_all"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -404,7 +403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C60548-35CF-4BDF-BF7E-7007C477EC71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -419,19 +418,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{786D9DD1-9CB9-4EF9-B986-6622DCEB1DD5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6044C16D-3079-4B4A-8448-072A32BA3463}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -444,13 +440,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -458,13 +454,13 @@
         <v>1880</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>97605</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -472,13 +468,13 @@
         <v>1880</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>118400</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,13 +482,13 @@
         <v>1881</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>98855</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,13 +496,13 @@
         <v>1881</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>108282</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,7 +510,7 @@
         <v>1882</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>115695</v>
@@ -525,7 +521,7 @@
         <v>1882</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>122031</v>
@@ -536,7 +532,7 @@
         <v>1883</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>120059</v>
@@ -547,7 +543,7 @@
         <v>1883</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>112477</v>
@@ -558,7 +554,7 @@
         <v>1884</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>137586</v>
@@ -569,7 +565,7 @@
         <v>1884</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>122738</v>
@@ -580,7 +576,7 @@
         <v>1885</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>141948</v>
@@ -591,7 +587,7 @@
         <v>1885</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>115945</v>
@@ -602,7 +598,7 @@
         <v>1886</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>153735</v>
@@ -613,7 +609,7 @@
         <v>1886</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>119041</v>
@@ -624,7 +620,7 @@
         <v>1887</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>155422</v>
@@ -635,7 +631,7 @@
         <v>1887</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>109313</v>
@@ -646,7 +642,7 @@
         <v>1888</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>189445</v>
@@ -657,7 +653,7 @@
         <v>1888</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>129906</v>
@@ -668,7 +664,7 @@
         <v>1889</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>189219</v>
@@ -679,7 +675,7 @@
         <v>1889</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>119032</v>
@@ -690,7 +686,7 @@
         <v>1890</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>201661</v>
@@ -701,7 +697,7 @@
         <v>1890</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>119701</v>
@@ -712,7 +708,7 @@
         <v>1891</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>196566</v>
@@ -723,7 +719,7 @@
         <v>1891</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>109265</v>
@@ -734,7 +730,7 @@
         <v>1892</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>224913</v>
@@ -745,7 +741,7 @@
         <v>1892</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>131453</v>
@@ -756,7 +752,7 @@
         <v>1893</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>225232</v>
@@ -767,7 +763,7 @@
         <v>1893</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>121041</v>
@@ -778,7 +774,7 @@
         <v>1894</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>235971</v>
@@ -789,7 +785,7 @@
         <v>1894</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>124893</v>
@@ -800,7 +796,7 @@
         <v>1895</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>247106</v>
@@ -811,7 +807,7 @@
         <v>1895</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>126643</v>
@@ -822,7 +818,7 @@
         <v>1896</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34">
         <v>251993</v>
@@ -833,7 +829,7 @@
         <v>1896</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <v>129071</v>
@@ -844,7 +840,7 @@
         <v>1897</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>248275</v>
@@ -855,7 +851,7 @@
         <v>1897</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37">
         <v>121942</v>
@@ -866,7 +862,7 @@
         <v>1898</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>274144</v>
@@ -877,7 +873,7 @@
         <v>1898</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39">
         <v>132104</v>
@@ -888,7 +884,7 @@
         <v>1899</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>247490</v>
@@ -899,7 +895,7 @@
         <v>1899</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>115193</v>
@@ -910,7 +906,7 @@
         <v>1900</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>317752</v>
@@ -921,7 +917,7 @@
         <v>1900</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>162133</v>
@@ -932,7 +928,7 @@
         <v>1901</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>254229</v>
@@ -943,7 +939,7 @@
         <v>1901</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>115595</v>
@@ -954,7 +950,7 @@
         <v>1902</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>280334</v>
@@ -965,7 +961,7 @@
         <v>1902</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <v>132750</v>
@@ -976,7 +972,7 @@
         <v>1903</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>278196</v>
@@ -987,7 +983,7 @@
         <v>1903</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>129326</v>
@@ -998,7 +994,7 @@
         <v>1904</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <v>292436</v>
@@ -1009,7 +1005,7 @@
         <v>1904</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>138508</v>
@@ -1020,7 +1016,7 @@
         <v>1905</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52">
         <v>309865</v>
@@ -1031,7 +1027,7 @@
         <v>1905</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53">
         <v>143238</v>
@@ -1042,7 +1038,7 @@
         <v>1906</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54">
         <v>313440</v>
@@ -1053,7 +1049,7 @@
         <v>1906</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55">
         <v>144071</v>
@@ -1064,7 +1060,7 @@
         <v>1907</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>337434</v>
@@ -1075,7 +1071,7 @@
         <v>1907</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57">
         <v>158587</v>
@@ -1086,7 +1082,7 @@
         <v>1908</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58">
         <v>354531</v>
@@ -1097,7 +1093,7 @@
         <v>1908</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59">
         <v>166368</v>
@@ -1108,7 +1104,7 @@
         <v>1909</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60">
         <v>368096</v>
@@ -1119,7 +1115,7 @@
         <v>1909</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C61">
         <v>176867</v>
@@ -1130,7 +1126,7 @@
         <v>1910</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <v>419526</v>
@@ -1141,7 +1137,7 @@
         <v>1910</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63">
         <v>208521</v>
@@ -1152,7 +1148,7 @@
         <v>1911</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64">
         <v>441818</v>
@@ -1163,7 +1159,7 @@
         <v>1911</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65">
         <v>241395</v>
@@ -1174,7 +1170,7 @@
         <v>1912</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>586712</v>
@@ -1185,7 +1181,7 @@
         <v>1912</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67">
         <v>451457</v>
@@ -1196,7 +1192,7 @@
         <v>1913</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68">
         <v>654913</v>
@@ -1207,7 +1203,7 @@
         <v>1913</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C69">
         <v>536247</v>
@@ -1218,7 +1214,7 @@
         <v>1914</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70">
         <v>796619</v>
@@ -1229,7 +1225,7 @@
         <v>1914</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C71">
         <v>683325</v>
@@ -1240,7 +1236,7 @@
         <v>1915</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72">
         <v>1023876</v>
@@ -1251,7 +1247,7 @@
         <v>1915</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C73">
         <v>880940</v>
@@ -1262,7 +1258,7 @@
         <v>1916</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74">
         <v>1085721</v>
@@ -1273,7 +1269,7 @@
         <v>1916</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75">
         <v>923257</v>
@@ -1284,7 +1280,7 @@
         <v>1917</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C76">
         <v>1123698</v>
@@ -1295,7 +1291,7 @@
         <v>1917</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C77">
         <v>959325</v>
@@ -1306,7 +1302,7 @@
         <v>1918</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78">
         <v>1202365</v>
@@ -1317,7 +1313,7 @@
         <v>1918</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C79">
         <v>1048674</v>
@@ -1328,7 +1324,7 @@
         <v>1919</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C80">
         <v>1174648</v>
@@ -1339,7 +1335,7 @@
         <v>1919</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C81">
         <v>1015337</v>
@@ -1350,7 +1346,7 @@
         <v>1920</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C82">
         <v>1244039</v>
@@ -1361,7 +1357,7 @@
         <v>1920</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C83">
         <v>1100817</v>
@@ -1372,7 +1368,7 @@
         <v>1921</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C84">
         <v>1279711</v>
@@ -1383,7 +1379,7 @@
         <v>1921</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85">
         <v>1137940</v>
@@ -1394,7 +1390,7 @@
         <v>1922</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C86">
         <v>1247556</v>
@@ -1405,7 +1401,7 @@
         <v>1922</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C87">
         <v>1125261</v>
@@ -1416,7 +1412,7 @@
         <v>1923</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88">
         <v>1252460</v>
@@ -1427,7 +1423,7 @@
         <v>1923</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>1132325</v>
@@ -1438,7 +1434,7 @@
         <v>1924</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C90">
         <v>1295706</v>
@@ -1449,7 +1445,7 @@
         <v>1924</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C91">
         <v>1169066</v>
@@ -1460,7 +1456,7 @@
         <v>1925</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92">
         <v>1263075</v>
@@ -1471,7 +1467,7 @@
         <v>1925</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93">
         <v>1151445</v>
@@ -1482,7 +1478,7 @@
         <v>1926</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C94">
         <v>1230152</v>
@@ -1493,7 +1489,7 @@
         <v>1926</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C95">
         <v>1145506</v>
@@ -1504,7 +1500,7 @@
         <v>1927</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C96">
         <v>1236397</v>
@@ -1515,7 +1511,7 @@
         <v>1927</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C97">
         <v>1161855</v>
@@ -1526,7 +1522,7 @@
         <v>1928</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C98">
         <v>1195463</v>
@@ -1537,7 +1533,7 @@
         <v>1928</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C99">
         <v>1141171</v>
@@ -1548,7 +1544,7 @@
         <v>1929</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C100">
         <v>1157521</v>
@@ -1559,7 +1555,7 @@
         <v>1929</v>
       </c>
       <c r="B101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C101">
         <v>1107538</v>
@@ -1570,7 +1566,7 @@
         <v>1930</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102">
         <v>1166423</v>
@@ -1581,7 +1577,7 @@
         <v>1930</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C103">
         <v>1129422</v>
@@ -1592,7 +1588,7 @@
         <v>1931</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C104">
         <v>1103625</v>
@@ -1603,7 +1599,7 @@
         <v>1931</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105">
         <v>1069568</v>
@@ -1614,7 +1610,7 @@
         <v>1932</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106">
         <v>1106222</v>
@@ -1625,7 +1621,7 @@
         <v>1932</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C107">
         <v>1074289</v>
@@ -1636,7 +1632,7 @@
         <v>1933</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C108">
         <v>1045936</v>
@@ -1647,7 +1643,7 @@
         <v>1933</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C109">
         <v>1020008</v>
@@ -1658,7 +1654,7 @@
         <v>1934</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C110">
         <v>1082225</v>
@@ -1669,7 +1665,7 @@
         <v>1934</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C111">
         <v>1061738</v>
@@ -1680,7 +1676,7 @@
         <v>1935</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112">
         <v>1086706</v>
@@ -1691,7 +1687,7 @@
         <v>1935</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C113">
         <v>1069387</v>
@@ -1702,7 +1698,7 @@
         <v>1936</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C114">
         <v>1077491</v>
@@ -1713,7 +1709,7 @@
         <v>1936</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>1064170</v>
@@ -1724,7 +1720,7 @@
         <v>1937</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116">
         <v>1101762</v>
@@ -1735,7 +1731,7 @@
         <v>1937</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C117">
         <v>1093483</v>
@@ -1746,7 +1742,7 @@
         <v>1938</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C118">
         <v>1141359</v>
@@ -1757,7 +1753,7 @@
         <v>1938</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C119">
         <v>1136302</v>
@@ -1768,7 +1764,7 @@
         <v>1939</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C120">
         <v>1134043</v>
@@ -1779,7 +1775,7 @@
         <v>1939</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C121">
         <v>1133162</v>
@@ -1790,7 +1786,7 @@
         <v>1940</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C122">
         <v>1181249</v>
@@ -1801,7 +1797,7 @@
         <v>1940</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C123">
         <v>1186022</v>
@@ -1812,7 +1808,7 @@
         <v>1941</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C124">
         <v>1245857</v>
@@ -1823,7 +1819,7 @@
         <v>1941</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C125">
         <v>1254654</v>
@@ -1834,7 +1830,7 @@
         <v>1942</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C126">
         <v>1390394</v>
@@ -1845,7 +1841,7 @@
         <v>1942</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C127">
         <v>1408070</v>
@@ -1856,7 +1852,7 @@
         <v>1943</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C128">
         <v>1435274</v>
@@ -1867,7 +1863,7 @@
         <v>1943</v>
       </c>
       <c r="B129" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C129">
         <v>1454311</v>
@@ -1878,7 +1874,7 @@
         <v>1944</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C130">
         <v>1366455</v>
@@ -1889,7 +1885,7 @@
         <v>1944</v>
       </c>
       <c r="B131" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C131">
         <v>1388968</v>
@@ -1900,7 +1896,7 @@
         <v>1945</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C132">
         <v>1346064</v>
@@ -1911,7 +1907,7 @@
         <v>1945</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C133">
         <v>1371285</v>
@@ -1922,7 +1918,7 @@
         <v>1946</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C134">
         <v>1612845</v>
@@ -1933,7 +1929,7 @@
         <v>1946</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C135">
         <v>1650220</v>
@@ -1944,7 +1940,7 @@
         <v>1947</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C136">
         <v>1817823</v>
@@ -1955,7 +1951,7 @@
         <v>1947</v>
       </c>
       <c r="B137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C137">
         <v>1857382</v>
@@ -1966,7 +1962,7 @@
         <v>1948</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C138">
         <v>1742576</v>
@@ -1977,7 +1973,7 @@
         <v>1948</v>
       </c>
       <c r="B139" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C139">
         <v>1782564</v>
@@ -1988,7 +1984,7 @@
         <v>1949</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C140">
         <v>1755492</v>
@@ -1999,7 +1995,7 @@
         <v>1949</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C141">
         <v>1801835</v>
@@ -2010,7 +2006,7 @@
         <v>1950</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C142">
         <v>1758618</v>
@@ -2021,7 +2017,7 @@
         <v>1950</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C143">
         <v>1819067</v>
@@ -2032,7 +2028,7 @@
         <v>1951</v>
       </c>
       <c r="B144" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C144">
         <v>1847277</v>
@@ -2043,7 +2039,7 @@
         <v>1951</v>
       </c>
       <c r="B145" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C145">
         <v>1911828</v>
@@ -2054,7 +2050,7 @@
         <v>1952</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C146">
         <v>1902276</v>
@@ -2065,7 +2061,7 @@
         <v>1952</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C147">
         <v>1974199</v>
@@ -2076,7 +2072,7 @@
         <v>1953</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C148">
         <v>1929099</v>
@@ -2087,7 +2083,7 @@
         <v>1953</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C149">
         <v>2001256</v>
@@ -2098,7 +2094,7 @@
         <v>1954</v>
       </c>
       <c r="B150" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C150">
         <v>1990839</v>
@@ -2109,7 +2105,7 @@
         <v>1954</v>
       </c>
       <c r="B151" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C151">
         <v>2068413</v>
@@ -2120,7 +2116,7 @@
         <v>1955</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152">
         <v>2004694</v>
@@ -2131,7 +2127,7 @@
         <v>1955</v>
       </c>
       <c r="B153" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C153">
         <v>2089594</v>
@@ -2142,7 +2138,7 @@
         <v>1956</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C154">
         <v>2059267</v>
@@ -2153,7 +2149,7 @@
         <v>1956</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C155">
         <v>2144575</v>
@@ -2164,7 +2160,7 @@
         <v>1957</v>
       </c>
       <c r="B156" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C156">
         <v>2097547</v>
@@ -2175,7 +2171,7 @@
         <v>1957</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C157">
         <v>2187459</v>
@@ -2186,7 +2182,7 @@
         <v>1958</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C158">
         <v>2065020</v>
@@ -2197,7 +2193,7 @@
         <v>1958</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C159">
         <v>2153039</v>
@@ -2208,7 +2204,7 @@
         <v>1959</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C160">
         <v>2078511</v>
@@ -2219,7 +2215,7 @@
         <v>1959</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C161">
         <v>2166256</v>
@@ -2230,7 +2226,7 @@
         <v>1960</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C162">
         <v>2079841</v>
@@ -2241,7 +2237,7 @@
         <v>1960</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C163">
         <v>2165696</v>
@@ -2252,7 +2248,7 @@
         <v>1961</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C164">
         <v>2076400</v>
@@ -2263,7 +2259,7 @@
         <v>1961</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C165">
         <v>2155956</v>
@@ -2274,7 +2270,7 @@
         <v>1962</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C166">
         <v>2026983</v>
@@ -2285,7 +2281,7 @@
         <v>1962</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C167">
         <v>2102051</v>
@@ -2296,7 +2292,7 @@
         <v>1963</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C168">
         <v>1987940</v>
@@ -2307,7 +2303,7 @@
         <v>1963</v>
       </c>
       <c r="B169" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C169">
         <v>2065187</v>
@@ -2318,7 +2314,7 @@
         <v>1964</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C170">
         <v>1957248</v>
@@ -2329,7 +2325,7 @@
         <v>1964</v>
       </c>
       <c r="B171" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C171">
         <v>2027330</v>
@@ -2340,7 +2336,7 @@
         <v>1965</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C172">
         <v>1827379</v>
@@ -2351,7 +2347,7 @@
         <v>1965</v>
       </c>
       <c r="B173" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C173">
         <v>1895210</v>
@@ -2362,7 +2358,7 @@
         <v>1966</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C174">
         <v>1755580</v>
@@ -2373,7 +2369,7 @@
         <v>1966</v>
       </c>
       <c r="B175" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C175">
         <v>1817912</v>
@@ -2384,7 +2380,7 @@
         <v>1967</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C176">
         <v>1716699</v>
@@ -2395,7 +2391,7 @@
         <v>1967</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C177">
         <v>1779774</v>
@@ -2406,7 +2402,7 @@
         <v>1968</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C178">
         <v>1709549</v>
@@ -2417,7 +2413,7 @@
         <v>1968</v>
       </c>
       <c r="B179" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C179">
         <v>1776069</v>
@@ -2428,7 +2424,7 @@
         <v>1969</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C180">
         <v>1762722</v>
@@ -2439,7 +2435,7 @@
         <v>1969</v>
       </c>
       <c r="B181" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C181">
         <v>1829979</v>
@@ -2450,7 +2446,7 @@
         <v>1970</v>
       </c>
       <c r="B182" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C182">
         <v>1831889</v>
@@ -2461,7 +2457,7 @@
         <v>1970</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C183">
         <v>1905622</v>
@@ -2472,7 +2468,7 @@
         <v>1971</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C184">
         <v>1752365</v>
@@ -2483,7 +2479,7 @@
         <v>1971</v>
       </c>
       <c r="B185" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C185">
         <v>1818381</v>
@@ -2494,7 +2490,7 @@
         <v>1972</v>
       </c>
       <c r="B186" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C186">
         <v>1612464</v>
@@ -2505,7 +2501,7 @@
         <v>1972</v>
       </c>
       <c r="B187" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C187">
         <v>1674675</v>
@@ -2516,7 +2512,7 @@
         <v>1973</v>
       </c>
       <c r="B188" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C188">
         <v>1554035</v>
@@ -2527,7 +2523,7 @@
         <v>1973</v>
       </c>
       <c r="B189" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C189">
         <v>1614211</v>
@@ -2538,7 +2534,7 @@
         <v>1974</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C190">
         <v>1566138</v>
@@ -2549,7 +2545,7 @@
         <v>1974</v>
       </c>
       <c r="B191" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C191">
         <v>1630740</v>
@@ -2560,7 +2556,7 @@
         <v>1975</v>
       </c>
       <c r="B192" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C192">
         <v>1560738</v>
@@ -2571,7 +2567,7 @@
         <v>1975</v>
       </c>
       <c r="B193" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C193">
         <v>1623029</v>
@@ -2582,7 +2578,7 @@
         <v>1976</v>
       </c>
       <c r="B194" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C194">
         <v>1571864</v>
@@ -2593,7 +2589,7 @@
         <v>1976</v>
       </c>
       <c r="B195" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C195">
         <v>1633225</v>
@@ -2604,7 +2600,7 @@
         <v>1977</v>
       </c>
       <c r="B196" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C196">
         <v>1644926</v>
@@ -2615,7 +2611,7 @@
         <v>1977</v>
       </c>
       <c r="B197" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C197">
         <v>1709859</v>
@@ -2626,7 +2622,7 @@
         <v>1978</v>
       </c>
       <c r="B198" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C198">
         <v>1643789</v>
@@ -2637,7 +2633,7 @@
         <v>1978</v>
       </c>
       <c r="B199" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C199">
         <v>1709099</v>
@@ -2648,7 +2644,7 @@
         <v>1979</v>
       </c>
       <c r="B200" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C200">
         <v>1723133</v>
@@ -2659,7 +2655,7 @@
         <v>1979</v>
       </c>
       <c r="B201" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C201">
         <v>1791825</v>
@@ -2670,7 +2666,7 @@
         <v>1980</v>
       </c>
       <c r="B202" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C202">
         <v>1780361</v>
@@ -2681,7 +2677,7 @@
         <v>1980</v>
       </c>
       <c r="B203" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C203">
         <v>1855024</v>
@@ -2692,7 +2688,7 @@
         <v>1981</v>
       </c>
       <c r="B204" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C204">
         <v>1788234</v>
@@ -2703,7 +2699,7 @@
         <v>1981</v>
       </c>
       <c r="B205" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C205">
         <v>1862416</v>
@@ -2714,7 +2710,7 @@
         <v>1982</v>
       </c>
       <c r="B206" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C206">
         <v>1813985</v>
@@ -2725,7 +2721,7 @@
         <v>1982</v>
       </c>
       <c r="B207" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C207">
         <v>1887126</v>
@@ -2736,7 +2732,7 @@
         <v>1983</v>
       </c>
       <c r="B208" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C208">
         <v>1789354</v>
@@ -2747,7 +2743,7 @@
         <v>1983</v>
       </c>
       <c r="B209" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C209">
         <v>1863331</v>
@@ -2758,7 +2754,7 @@
         <v>1984</v>
       </c>
       <c r="B210" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C210">
         <v>1802890</v>
@@ -2769,7 +2765,7 @@
         <v>1984</v>
       </c>
       <c r="B211" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C211">
         <v>1876225</v>
@@ -2780,7 +2776,7 @@
         <v>1985</v>
       </c>
       <c r="B212" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C212">
         <v>1845903</v>
@@ -2791,7 +2787,7 @@
         <v>1985</v>
       </c>
       <c r="B213" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C213">
         <v>1923822</v>
@@ -2802,7 +2798,7 @@
         <v>1986</v>
       </c>
       <c r="B214" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C214">
         <v>1845046</v>
@@ -2813,7 +2809,7 @@
         <v>1986</v>
       </c>
       <c r="B215" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C215">
         <v>1920958</v>
@@ -2824,7 +2820,7 @@
         <v>1987</v>
       </c>
       <c r="B216" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C216">
         <v>1873831</v>
@@ -2835,7 +2831,7 @@
         <v>1987</v>
       </c>
       <c r="B217" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C217">
         <v>1949471</v>
@@ -2846,7 +2842,7 @@
         <v>1988</v>
       </c>
       <c r="B218" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C218">
         <v>1922580</v>
@@ -2857,7 +2853,7 @@
         <v>1988</v>
       </c>
       <c r="B219" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C219">
         <v>2001329</v>
@@ -2868,7 +2864,7 @@
         <v>1989</v>
       </c>
       <c r="B220" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C220">
         <v>1991890</v>
@@ -2879,7 +2875,7 @@
         <v>1989</v>
       </c>
       <c r="B221" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C221">
         <v>2095455</v>
@@ -2890,7 +2886,7 @@
         <v>1990</v>
       </c>
       <c r="B222" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C222">
         <v>2053962</v>
@@ -2901,7 +2897,7 @@
         <v>1990</v>
       </c>
       <c r="B223" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C223">
         <v>2151160</v>
@@ -2912,7 +2908,7 @@
         <v>1991</v>
       </c>
       <c r="B224" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C224">
         <v>2033116</v>
@@ -2923,7 +2919,7 @@
         <v>1991</v>
       </c>
       <c r="B225" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C225">
         <v>2119192</v>
@@ -2934,7 +2930,7 @@
         <v>1992</v>
       </c>
       <c r="B226" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C226">
         <v>2004297</v>
@@ -2945,7 +2941,7 @@
         <v>1992</v>
       </c>
       <c r="B227" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C227">
         <v>2098620</v>
@@ -2956,7 +2952,7 @@
         <v>1993</v>
       </c>
       <c r="B228" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C228">
         <v>1971175</v>
@@ -2967,7 +2963,7 @@
         <v>1993</v>
       </c>
       <c r="B229" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C229">
         <v>2064960</v>
@@ -2978,7 +2974,7 @@
         <v>1994</v>
       </c>
       <c r="B230" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C230">
         <v>1949024</v>
@@ -2989,7 +2985,7 @@
         <v>1994</v>
       </c>
       <c r="B231" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C231">
         <v>2037946</v>
@@ -3000,7 +2996,7 @@
         <v>1995</v>
       </c>
       <c r="B232" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C232">
         <v>1921218</v>
@@ -3011,7 +3007,7 @@
         <v>1995</v>
       </c>
       <c r="B233" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C233">
         <v>2010995</v>
@@ -3022,7 +3018,7 @@
         <v>1996</v>
       </c>
       <c r="B234" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C234">
         <v>1916882</v>
@@ -3033,7 +3029,7 @@
         <v>1996</v>
       </c>
       <c r="B235" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C235">
         <v>2003372</v>
@@ -3044,7 +3040,7 @@
         <v>1997</v>
       </c>
       <c r="B236" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C236">
         <v>1908808</v>
@@ -3055,7 +3051,7 @@
         <v>1997</v>
       </c>
       <c r="B237" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C237">
         <v>1997337</v>
@@ -3066,7 +3062,7 @@
         <v>1998</v>
       </c>
       <c r="B238" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C238">
         <v>1938008</v>
@@ -3077,7 +3073,7 @@
         <v>1998</v>
       </c>
       <c r="B239" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C239">
         <v>2027136</v>
@@ -3088,7 +3084,7 @@
         <v>1999</v>
       </c>
       <c r="B240" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C240">
         <v>1946204</v>
@@ -3099,7 +3095,7 @@
         <v>1999</v>
       </c>
       <c r="B241" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C241">
         <v>2038346</v>
@@ -3110,7 +3106,7 @@
         <v>2000</v>
       </c>
       <c r="B242" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C242">
         <v>1994881</v>
@@ -3121,7 +3117,7 @@
         <v>2000</v>
       </c>
       <c r="B243" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C243">
         <v>2087391</v>
@@ -3132,7 +3128,7 @@
         <v>2001</v>
       </c>
       <c r="B244" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C244">
         <v>1980040</v>
@@ -3143,7 +3139,7 @@
         <v>2001</v>
       </c>
       <c r="B245" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C245">
         <v>2067422</v>
@@ -3154,7 +3150,7 @@
         <v>2002</v>
       </c>
       <c r="B246" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C246">
         <v>1973957</v>
@@ -3165,7 +3161,7 @@
         <v>2002</v>
       </c>
       <c r="B247" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C247">
         <v>2065531</v>
@@ -3176,7 +3172,7 @@
         <v>2003</v>
       </c>
       <c r="B248" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C248">
         <v>2005406</v>
@@ -3187,7 +3183,7 @@
         <v>2003</v>
       </c>
       <c r="B249" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C249">
         <v>2100052</v>
@@ -3198,7 +3194,7 @@
         <v>2004</v>
       </c>
       <c r="B250" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C250">
         <v>2016585</v>
@@ -3209,7 +3205,7 @@
         <v>2004</v>
       </c>
       <c r="B251" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C251">
         <v>2112190</v>
@@ -3220,7 +3216,7 @@
         <v>2005</v>
       </c>
       <c r="B252" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C252">
         <v>2028174</v>
@@ -3231,7 +3227,7 @@
         <v>2005</v>
       </c>
       <c r="B253" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C253">
         <v>2126034</v>
@@ -3242,7 +3238,7 @@
         <v>2006</v>
       </c>
       <c r="B254" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C254">
         <v>2089049</v>
@@ -3253,7 +3249,7 @@
         <v>2006</v>
       </c>
       <c r="B255" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C255">
         <v>2190837</v>
@@ -3264,7 +3260,7 @@
         <v>2007</v>
       </c>
       <c r="B256" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C256">
         <v>2114797</v>
@@ -3275,7 +3271,7 @@
         <v>2007</v>
       </c>
       <c r="B257" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C257">
         <v>2213423</v>
@@ -3286,7 +3282,7 @@
         <v>2008</v>
       </c>
       <c r="B258" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C258">
         <v>2080929</v>
@@ -3297,7 +3293,7 @@
         <v>2008</v>
       </c>
       <c r="B259" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C259">
         <v>2178453</v>
@@ -3308,7 +3304,7 @@
         <v>2009</v>
       </c>
       <c r="B260" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C260">
         <v>2022977</v>
@@ -3319,7 +3315,7 @@
         <v>2009</v>
       </c>
       <c r="B261" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C261">
         <v>2118953</v>
@@ -3330,7 +3326,7 @@
         <v>2010</v>
       </c>
       <c r="B262" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C262">
         <v>1958284</v>
@@ -3341,7 +3337,7 @@
         <v>2010</v>
       </c>
       <c r="B263" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C263">
         <v>2052122</v>
@@ -3352,7 +3348,7 @@
         <v>2011</v>
       </c>
       <c r="B264" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C264">
         <v>1935047</v>
@@ -3363,7 +3359,7 @@
         <v>2011</v>
       </c>
       <c r="B265" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C265">
         <v>2028589</v>
@@ -3374,7 +3370,7 @@
         <v>2012</v>
       </c>
       <c r="B266" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C266">
         <v>1936239</v>
@@ -3385,7 +3381,7 @@
         <v>2012</v>
       </c>
       <c r="B267" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C267">
         <v>2025890</v>
@@ -3396,7 +3392,7 @@
         <v>2013</v>
       </c>
       <c r="B268" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C268">
         <v>1923856</v>
@@ -3407,7 +3403,7 @@
         <v>2013</v>
       </c>
       <c r="B269" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C269">
         <v>2016731</v>
@@ -3418,7 +3414,7 @@
         <v>2014</v>
       </c>
       <c r="B270" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C270">
         <v>1951652</v>
@@ -3429,7 +3425,7 @@
         <v>2014</v>
       </c>
       <c r="B271" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C271">
         <v>2044378</v>
@@ -3440,7 +3436,7 @@
         <v>2015</v>
       </c>
       <c r="B272" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C272">
         <v>1945317</v>
@@ -3451,7 +3447,7 @@
         <v>2015</v>
       </c>
       <c r="B273" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C273">
         <v>2038331</v>
@@ -3462,7 +3458,7 @@
         <v>2016</v>
       </c>
       <c r="B274" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C274">
         <v>1928438</v>
@@ -3473,7 +3469,7 @@
         <v>2016</v>
       </c>
       <c r="B275" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C275">
         <v>2017790</v>
@@ -3484,7 +3480,7 @@
         <v>2017</v>
       </c>
       <c r="B276" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C276">
         <v>1874899</v>
@@ -3495,7 +3491,7 @@
         <v>2017</v>
       </c>
       <c r="B277" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C277">
         <v>1963290</v>

</xml_diff>